<commit_message>
making sure we dont lose any samples in the pipeline due to _ in names, etc
</commit_message>
<xml_diff>
--- a/data/mapping_file2.xlsx
+++ b/data/mapping_file2.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="89">
   <si>
     <t>SampleID</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>KI17aFL280</t>
+  </si>
+  <si>
+    <t>KI115cFMD501</t>
+  </si>
+  <si>
+    <t>2015Jul</t>
   </si>
 </sst>
 </file>
@@ -649,10 +655,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A10798-5A7A-4B73-8DF8-B9CADD7571C1}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2929,6 +2936,38 @@
         <v>13</v>
       </c>
     </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>87</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>783</v>
+      </c>
+      <c r="D72" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" t="s">
+        <v>88</v>
+      </c>
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" t="s">
+        <v>14</v>
+      </c>
+      <c r="H72">
+        <v>34</v>
+      </c>
+      <c r="I72" t="s">
+        <v>15</v>
+      </c>
+      <c r="J72" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>